<commit_message>
update open source review table for fledge iot and fledge power
</commit_message>
<xml_diff>
--- a/Open-Source_Gateway_Review.xlsx
+++ b/Open-Source_Gateway_Review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/github/orxa/comms_gateway/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6250673D-C9EF-024B-B0B5-23AE7512C0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079C5B00-6ED1-B74F-9894-AF943FEC88CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="1420" windowWidth="28040" windowHeight="17440" xr2:uid="{BACD2997-F745-254E-A4FA-F0BBCA75FF79}"/>
+    <workbookView xWindow="2680" yWindow="1320" windowWidth="33580" windowHeight="18920" xr2:uid="{BACD2997-F745-254E-A4FA-F0BBCA75FF79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>FledgeIoT</t>
   </si>
@@ -62,9 +62,6 @@
     <t>MQTT</t>
   </si>
   <si>
-    <t>HTTP REST</t>
-  </si>
-  <si>
     <t>IEC 104</t>
   </si>
   <si>
@@ -89,30 +86,12 @@
     <t>License</t>
   </si>
   <si>
-    <t>HTTP API</t>
-  </si>
-  <si>
-    <t>Latest reading</t>
-  </si>
-  <si>
-    <t>GUI</t>
-  </si>
-  <si>
     <t>Streaming output</t>
   </si>
   <si>
-    <t>Min / Max / Avg readings</t>
-  </si>
-  <si>
     <t>Expressions</t>
   </si>
   <si>
-    <t>Alarms</t>
-  </si>
-  <si>
-    <t>Docker</t>
-  </si>
-  <si>
     <t>High Availability</t>
   </si>
   <si>
@@ -123,13 +102,103 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Export config</t>
+  </si>
+  <si>
+    <t>Forks</t>
+  </si>
+  <si>
+    <t>Stars</t>
+  </si>
+  <si>
+    <t>Owner / Maintainer</t>
+  </si>
+  <si>
+    <t>Commits</t>
+  </si>
+  <si>
+    <t>ThingsBoard, Inc</t>
+  </si>
+  <si>
+    <t>OpenJS Foundation</t>
+  </si>
+  <si>
+    <t>https://lfedge.org/projects/fledge/</t>
+  </si>
+  <si>
+    <t>Linux Foundation (Edge)</t>
+  </si>
+  <si>
+    <t>Linux Foundation (Energy)</t>
+  </si>
+  <si>
+    <t>https://github.com/fledge-iot/fledge</t>
+  </si>
+  <si>
+    <t>https://fledge-iot.readthedocs.io/en/latest/</t>
+  </si>
+  <si>
+    <t>11k</t>
+  </si>
+  <si>
+    <t>Apache-2.0</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>REST Admin API</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Real time latest measurement</t>
+  </si>
+  <si>
+    <t>Min / Max / Avg measurement</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>HTTP output</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Docker / Docker Compose</t>
+  </si>
+  <si>
+    <t>https://github.com/fledge-power/fledgepower-deployment</t>
+  </si>
+  <si>
+    <t>https://wiki.lfenergy.org/display/FLED/FledgePower</t>
+  </si>
+  <si>
+    <t>https://lfenergy.org/projects/fledgepower/</t>
+  </si>
+  <si>
+    <t>0.5k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,6 +216,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -174,10 +249,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,23 +589,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2EAB25-C928-3341-89ED-44657C57F4F2}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -549,147 +626,419 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3">
+        <v>120</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{96A9763D-C0E2-8D45-BC80-689A55BDD42A}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{1BF0359F-C54D-104D-9FB6-7AA9707E55E2}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{ECDB0EC1-F224-214E-A62B-FD35293D8D96}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{1A013F5A-064F-FF45-85DB-9A7A2A2DD2D9}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{9CECE43A-3F2B-CA45-8325-1F8241DFACE3}"/>
+    <hyperlink ref="B12" r:id="rId6" xr:uid="{2D27207F-1652-1C4D-961C-85B0C585F96C}"/>
+    <hyperlink ref="B14" r:id="rId7" xr:uid="{082F432B-8214-7B4B-B714-D59944C921AA}"/>
+    <hyperlink ref="B15" r:id="rId8" xr:uid="{16F2E032-4978-7A45-91A9-3AF8FE4B0CEF}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{00232F19-4398-BA42-B301-BCC5F46F185C}"/>
+    <hyperlink ref="B21" r:id="rId10" location="get-asset-reading" xr:uid="{462A8A9C-69C3-DE4C-98F5-D6D43EF9FBBD}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{EECBDFA4-974D-2F49-9E78-9CCC258A8DD7}"/>
+    <hyperlink ref="B19" r:id="rId12" xr:uid="{2CB5AE44-F0B0-4844-90BC-2F28F9F92EAB}"/>
+    <hyperlink ref="B20" r:id="rId13" xr:uid="{B0C240AE-0D37-D64D-8E54-872CBABE3376}"/>
+    <hyperlink ref="B22" r:id="rId14" location="get-asset-reading-summary" xr:uid="{D1C4FC8C-FE2A-D84E-AE02-907CE2E52075}"/>
+    <hyperlink ref="B23" r:id="rId15" xr:uid="{EE082293-6DEB-5D44-B88A-2755C79817EA}"/>
+    <hyperlink ref="B24" r:id="rId16" xr:uid="{366539D7-477E-6F47-82A7-B7B19E8CDB68}"/>
+    <hyperlink ref="B25" r:id="rId17" xr:uid="{256F9807-8E43-C04F-BD46-73ABC1B7FC60}"/>
+    <hyperlink ref="B27" r:id="rId18" location="plugin-information" xr:uid="{000199AB-9ECF-6642-A8C5-667FF13DBAD4}"/>
+    <hyperlink ref="B28" r:id="rId19" xr:uid="{1A172B30-512F-764B-9DDB-9BBA3159D756}"/>
+    <hyperlink ref="B29" r:id="rId20" xr:uid="{4BE3A052-96AC-794B-8BFF-037B00AFE724}"/>
+    <hyperlink ref="C10" r:id="rId21" xr:uid="{D40023D2-BAD7-B045-B86A-CE92EFA6BD5D}"/>
+    <hyperlink ref="C17" r:id="rId22" xr:uid="{F622A56F-BC29-204D-9AC2-F5B98D884FBD}"/>
+    <hyperlink ref="C21" r:id="rId23" location="get-asset-reading" xr:uid="{EC7284E4-1F25-1344-8C38-5392885331CA}"/>
+    <hyperlink ref="C18" r:id="rId24" xr:uid="{004DEA75-BD44-8040-BCFA-D91FBCCAF70A}"/>
+    <hyperlink ref="C19" r:id="rId25" xr:uid="{19091A1B-EC9B-6144-BCFF-DCEDEDF647DA}"/>
+    <hyperlink ref="C22" r:id="rId26" location="get-asset-reading-summary" xr:uid="{5BCC24EC-D42F-5544-9A83-A211B92C20F1}"/>
+    <hyperlink ref="C23" r:id="rId27" xr:uid="{BDBB21FA-AB01-7E44-AD78-AC96A21B7A15}"/>
+    <hyperlink ref="C24" r:id="rId28" xr:uid="{CB515FCE-D386-F64C-ACB8-220B4219EF5C}"/>
+    <hyperlink ref="C25" r:id="rId29" xr:uid="{AD1AFFCC-D7D4-4040-A228-CA76792C0127}"/>
+    <hyperlink ref="C27" r:id="rId30" location="plugin-information" xr:uid="{560FB469-4AAC-884A-BD7D-4FA2FA0835C7}"/>
+    <hyperlink ref="C28" r:id="rId31" xr:uid="{A88FA9D5-EA78-3340-A7C8-086C6A80F45A}"/>
+    <hyperlink ref="C29" r:id="rId32" xr:uid="{8B82DD2E-7088-5F4D-BC0E-371FC5FFE415}"/>
+    <hyperlink ref="B13" r:id="rId33" display="✓" xr:uid="{BB45D5C3-3AC9-6942-A4FD-D22D69B5AA2A}"/>
+    <hyperlink ref="C13" r:id="rId34" xr:uid="{01A73ED8-BEAB-7B4E-AAF4-2F1CD8B400DF}"/>
+    <hyperlink ref="C16" r:id="rId35" xr:uid="{2F4A997D-F1B8-AA4D-9D45-4ED597F93F96}"/>
+    <hyperlink ref="C4" r:id="rId36" xr:uid="{329A7A39-0A97-3A4F-8BF1-9381DEFED7B7}"/>
+    <hyperlink ref="C5" r:id="rId37" xr:uid="{8A013E14-DC29-A641-92EA-028F42A8FF9F}"/>
+    <hyperlink ref="C3" r:id="rId38" xr:uid="{FAAEA543-78A3-2944-AD05-EB80D6F064E2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update excel table of open source comms gateways
</commit_message>
<xml_diff>
--- a/Open-Source_Gateway_Review.xlsx
+++ b/Open-Source_Gateway_Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/github/orxa/comms_gateway/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCB9DA0-A174-2940-9DB3-66B6919822F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC1224A-CB1E-C346-B17F-C0218BE6ECEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1320" windowWidth="33580" windowHeight="18920" xr2:uid="{BACD2997-F745-254E-A4FA-F0BBCA75FF79}"/>
+    <workbookView xWindow="760" yWindow="1180" windowWidth="26940" windowHeight="16300" xr2:uid="{BACD2997-F745-254E-A4FA-F0BBCA75FF79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>FledgeIoT</t>
   </si>
@@ -192,13 +192,31 @@
   </si>
   <si>
     <t>0.5k</t>
+  </si>
+  <si>
+    <t>https://lfedge.org/projects/edgex-foundry/</t>
+  </si>
+  <si>
+    <t>https://github.com/edgexfoundry/edgex-go</t>
+  </si>
+  <si>
+    <t>1.3k</t>
+  </si>
+  <si>
+    <t>4.5k</t>
+  </si>
+  <si>
+    <t>https://docs.edgexfoundry.org/3.1/</t>
+  </si>
+  <si>
+    <t>https://docs.edgexfoundry.org/3.1/microservices/device/services/device-modbus/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,6 +245,14 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,11 +275,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,19 +628,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2EAB25-C928-3341-89ED-44657C57F4F2}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -627,7 +667,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -637,7 +677,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>27</v>
@@ -648,46 +688,55 @@
       <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="D3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="D5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="3">
@@ -696,10 +745,13 @@
       <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="D6" s="3">
+        <v>481</v>
+      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="3">
@@ -708,10 +760,13 @@
       <c r="C7" s="3">
         <v>4</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -720,10 +775,13 @@
       <c r="C8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -732,37 +790,46 @@
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="D10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -771,166 +838,166 @@
       <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="2"/>
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="2"/>
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="2"/>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="2"/>
+      <c r="B18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="2"/>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="2"/>
+      <c r="B21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="2"/>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="2"/>
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="2"/>
+      <c r="B24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="2"/>
+      <c r="B25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -939,64 +1006,64 @@
       <c r="C26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="2"/>
+      <c r="B27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="2"/>
+      <c r="B28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H29" s="2"/>
+      <c r="B29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H30" s="2"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H32" s="2"/>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H33" s="2"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34" s="2"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H35" s="2"/>
+      <c r="H35" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1036,6 +1103,10 @@
     <hyperlink ref="C4" r:id="rId34" xr:uid="{329A7A39-0A97-3A4F-8BF1-9381DEFED7B7}"/>
     <hyperlink ref="C5" r:id="rId35" xr:uid="{8A013E14-DC29-A641-92EA-028F42A8FF9F}"/>
     <hyperlink ref="C3" r:id="rId36" xr:uid="{FAAEA543-78A3-2944-AD05-EB80D6F064E2}"/>
+    <hyperlink ref="D3" r:id="rId37" xr:uid="{DB2E1188-6713-694D-A630-813C63814751}"/>
+    <hyperlink ref="D4" r:id="rId38" xr:uid="{FF1F54F4-F9EA-9145-A4C2-E778BE4FD7EE}"/>
+    <hyperlink ref="D5" r:id="rId39" xr:uid="{6C97B91E-8285-0C46-968D-99864DCCE24A}"/>
+    <hyperlink ref="D10" r:id="rId40" xr:uid="{4D3AFA39-F27A-0F42-8E37-F0AD7DF186C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>